<commit_message>
THis is last commit of 2023
</commit_message>
<xml_diff>
--- a/src/test/java/Day100/caldata2.xlsx
+++ b/src/test/java/Day100/caldata2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
   <si>
     <t>Initial Deposit amout</t>
   </si>
@@ -174,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -195,6 +195,11 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -565,7 +570,7 @@
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s" s="35">
+      <c r="G2" t="s" s="40">
         <v>17</v>
       </c>
     </row>
@@ -588,7 +593,7 @@
       <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s" s="36">
+      <c r="G3" t="s" s="41">
         <v>17</v>
       </c>
     </row>
@@ -611,7 +616,7 @@
       <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s" s="37">
+      <c r="G4" t="s" s="42">
         <v>17</v>
       </c>
     </row>
@@ -634,7 +639,7 @@
       <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" t="s" s="38">
+      <c r="G5" t="s" s="43">
         <v>17</v>
       </c>
     </row>
@@ -657,7 +662,7 @@
       <c r="F6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s" s="39">
+      <c r="G6" t="s" s="44">
         <v>18</v>
       </c>
     </row>

</xml_diff>